<commit_message>
fix lassa virus, genbank accession extraction
</commit_message>
<xml_diff>
--- a/Pubmed/Lassa/Lassa_AI_search_checked.xlsx
+++ b/Pubmed/Lassa/Lassa_AI_search_checked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/HIVDB/GenBankRefs/Pubmed/Lassa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDC532C-0530-D544-8B86-F271759C4652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F125DD97-92B6-344F-906E-270B85C19958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="1560" windowWidth="20100" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10000" yWindow="1060" windowWidth="20100" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="197">
   <si>
     <t>RefID</t>
   </si>
@@ -585,15 +585,6 @@
   </si>
   <si>
     <t>https://www.biorxiv.org/content/10.1101/616466v1.full</t>
-  </si>
-  <si>
-    <t>36992478, 34634087</t>
-  </si>
-  <si>
-    <t>30606844, 31413134</t>
-  </si>
-  <si>
-    <t>30050872, 31588039</t>
   </si>
   <si>
     <t>Double check</t>
@@ -1091,7 +1082,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C37"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1121,13 +1112,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1138,7 +1129,7 @@
         <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -1202,7 +1193,7 @@
         <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1213,7 +1204,7 @@
         <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D5" t="s">
         <v>49</v>
@@ -1231,7 +1222,7 @@
         <v>52</v>
       </c>
       <c r="I5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1266,7 +1257,7 @@
         <v>93</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D7" t="s">
         <v>94</v>
@@ -1290,7 +1281,7 @@
         <v>149</v>
       </c>
       <c r="C8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D8" t="s">
         <v>150</v>
@@ -1306,7 +1297,7 @@
         <v>152</v>
       </c>
       <c r="I8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1317,7 +1308,7 @@
         <v>102</v>
       </c>
       <c r="C9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D9" t="s">
         <v>103</v>
@@ -1335,7 +1326,7 @@
         <v>105</v>
       </c>
       <c r="I9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1346,7 +1337,7 @@
         <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D10" t="s">
         <v>44</v>
@@ -1364,7 +1355,7 @@
         <v>47</v>
       </c>
       <c r="I10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1391,7 +1382,7 @@
         <v>38</v>
       </c>
       <c r="I11" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1418,7 +1409,7 @@
         <v>42</v>
       </c>
       <c r="I12" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1447,7 +1438,7 @@
         <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1458,7 +1449,7 @@
         <v>123</v>
       </c>
       <c r="C14" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D14" t="s">
         <v>124</v>
@@ -1482,7 +1473,7 @@
         <v>153</v>
       </c>
       <c r="C15" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D15" t="s">
         <v>154</v>
@@ -1493,14 +1484,14 @@
       <c r="F15" t="s">
         <v>155</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>168</v>
+      <c r="G15" s="2">
+        <v>31588039</v>
       </c>
       <c r="H15" t="s">
         <v>156</v>
       </c>
       <c r="I15" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1511,7 +1502,7 @@
         <v>137</v>
       </c>
       <c r="C16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D16" t="s">
         <v>138</v>
@@ -1529,7 +1520,7 @@
         <v>140</v>
       </c>
       <c r="I16" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1540,7 +1531,7 @@
         <v>119</v>
       </c>
       <c r="C17" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D17" t="s">
         <v>120</v>
@@ -1558,7 +1549,7 @@
         <v>122</v>
       </c>
       <c r="I17" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1587,7 +1578,7 @@
         <v>63</v>
       </c>
       <c r="I18" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1598,7 +1589,7 @@
         <v>98</v>
       </c>
       <c r="C19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D19" t="s">
         <v>99</v>
@@ -1616,7 +1607,7 @@
         <v>101</v>
       </c>
       <c r="I19" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1651,7 +1642,7 @@
         <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D21" t="s">
         <v>142</v>
@@ -1662,14 +1653,14 @@
       <c r="F21" t="s">
         <v>143</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>167</v>
+      <c r="G21" s="2">
+        <v>30606844</v>
       </c>
       <c r="H21" t="s">
         <v>144</v>
       </c>
       <c r="I21" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1680,7 +1671,7 @@
         <v>115</v>
       </c>
       <c r="C22" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D22" t="s">
         <v>116</v>
@@ -1698,7 +1689,7 @@
         <v>118</v>
       </c>
       <c r="I22" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1709,7 +1700,7 @@
         <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D23" t="s">
         <v>80</v>
@@ -1733,7 +1724,7 @@
         <v>111</v>
       </c>
       <c r="C24" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D24" t="s">
         <v>112</v>
@@ -1751,7 +1742,7 @@
         <v>114</v>
       </c>
       <c r="I24" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1762,7 +1753,7 @@
         <v>106</v>
       </c>
       <c r="C25" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D25" t="s">
         <v>107</v>
@@ -1780,7 +1771,7 @@
         <v>110</v>
       </c>
       <c r="I25" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1815,7 +1806,7 @@
         <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D27" t="s">
         <v>54</v>
@@ -1826,14 +1817,14 @@
       <c r="F27" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>166</v>
+      <c r="G27" s="2">
+        <v>34634087</v>
       </c>
       <c r="H27" t="s">
         <v>57</v>
       </c>
       <c r="I27" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1868,7 +1859,7 @@
         <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D29" t="s">
         <v>85</v>
@@ -1886,7 +1877,7 @@
         <v>87</v>
       </c>
       <c r="I29" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1897,7 +1888,7 @@
         <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D30" t="s">
         <v>75</v>
@@ -1913,7 +1904,7 @@
         <v>78</v>
       </c>
       <c r="I30" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1924,7 +1915,7 @@
         <v>145</v>
       </c>
       <c r="C31" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D31" t="s">
         <v>146</v>
@@ -1942,7 +1933,7 @@
         <v>148</v>
       </c>
       <c r="I31" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1953,7 +1944,7 @@
         <v>128</v>
       </c>
       <c r="C32" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D32" t="s">
         <v>129</v>
@@ -1969,7 +1960,7 @@
         <v>132</v>
       </c>
       <c r="I32" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -1980,7 +1971,7 @@
         <v>161</v>
       </c>
       <c r="C33" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D33" t="s">
         <v>162</v>
@@ -2004,7 +1995,7 @@
         <v>157</v>
       </c>
       <c r="C34" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D34" t="s">
         <v>158</v>
@@ -2022,7 +2013,7 @@
         <v>160</v>
       </c>
       <c r="I34" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -2057,7 +2048,7 @@
         <v>133</v>
       </c>
       <c r="C36" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D36" t="s">
         <v>134</v>
@@ -2083,7 +2074,7 @@
         <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D37" t="s">
         <v>65</v>
@@ -2101,7 +2092,7 @@
         <v>68</v>
       </c>
       <c r="I37" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>